<commit_message>
local environment 20221003 1341
</commit_message>
<xml_diff>
--- a/OnCall/2022-09-26 to 2022-10-02/On Call Report.xlsx
+++ b/OnCall/2022-09-26 to 2022-10-02/On Call Report.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\WIP\OnCall\2022-09-26 to 2022-10-02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C0BAF-1F8B-4586-A6C7-072EF77F120E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D597EE1D-FDE8-41E5-969A-4DE27189BAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
+    <workbookView xWindow="17085" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{811B3618-D1A8-47C6-AF60-49222DFFA8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Job Failures" sheetId="1" r:id="rId1"/>
     <sheet name="Application Dead Locks" sheetId="3" r:id="rId2"/>
     <sheet name="Dead Locks" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Dead Locks'!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="78">
   <si>
     <t>SQL08</t>
   </si>
@@ -169,6 +172,108 @@
   </si>
   <si>
     <t>Datafeed - eCommerce - SPS - Incoming</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DS-TREZMANH</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.InvWarehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WMS; WMS (victim)</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletItem; WarehouseCompany100.dbo.tblPalletReserved</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletItem</t>
+  </si>
+  <si>
+    <t>tempdb.sys.sysschobjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1-MN-SC2909-PC (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\Ben (victim); HASSIET_SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TALEND (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQL_Talend (victim); ASHLIEW_SYSPRO</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.CusSorMaster+; SysproCompany100.dbo.SorMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEPHANIET_SYSPRO; ALYSSAC_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.GenJournalDetail</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletReserved; WarehouseCompany100.dbo.tblPickingSlipItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EWsys; EWsys (victim)</t>
+  </si>
+  <si>
+    <t>EPX.dbo.P_WORK_ITEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WSUS; WSUS (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SentryOneUser; SentryOneUser (victim)</t>
+  </si>
+  <si>
+    <t>SentryOne.dbo.EventSourceHistory; SentryOne.dbo.MetaHistorySqlServerTraceLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARGARETH_SYSPRO; ASHLIEW_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.ArControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEV-JUSTINP (victim); 7SYSPRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\adm_justinp (victim); SUMMERCLASSICS\EcatSalesOrderImport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STEPHANIET_SYSPRO; ELLENM_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DWAYNEP_SYSPRO; DS-ZANQUESEJ (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.SorDetail</t>
+  </si>
+  <si>
+    <t>WarehouseCompany100.dbo.tblPalletReserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQLREPORTING; DESKTOP-IGRF887 (victim)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUMMERCLASSICS\SqlAgentUser; RJAYARAM (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.ArTrnSummary; SysproCompany100.dbo.SorMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEV-THESG; SQLREPORTING (victim)</t>
+  </si>
+  <si>
+    <t>tempdb.dbo.#A010EBEC; tempdb.dbo.#BC405B08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUEB_SYSPRO; LEEE_SYSPRO (victim)</t>
+  </si>
+  <si>
+    <t>SysproCompany100.dbo.GenControl</t>
   </si>
 </sst>
 </file>
@@ -540,21 +645,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B947EB8-A820-4DB1-A77B-9E8A150A9680}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="172.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="172.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -570,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -578,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -586,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -594,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -602,7 +707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -610,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -620,7 +725,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,7 +751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -675,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -704,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -733,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -762,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -791,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -820,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -849,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -878,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -907,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -936,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -965,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -994,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1023,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1052,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1081,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1110,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1139,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1168,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1197,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1255,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1294,16 +1399,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CE61EA-4898-4378-A30B-E952358415B0}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="118.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="118.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1318,7 +1423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1326,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1334,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1342,7 +1447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1350,7 +1455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1358,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1366,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1374,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1390,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1398,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1416,20 +1521,20 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD26"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1452,82 +1557,587 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44834.563924108799</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>12885</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>44831.579732986109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3">
+        <v>12867</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>44830.632940243057</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4">
+        <v>12861</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6">
+        <v>44832.565205937499</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>12874</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>44834.556142789355</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>12884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>44830.377649074071</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7">
+        <v>12858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>44832.473534143515</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8">
+        <v>12872</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <v>44834.551571412034</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9">
+        <v>12882</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <v>44830.377735960647</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>12859</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>44832.492029398149</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>12873</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <v>44834.556084837961</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12">
+        <v>12883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <v>44832.454831053241</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13">
+        <v>12870</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6">
+        <v>44833.456100659721</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14">
+        <v>12881</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6">
+        <v>44833.438969710645</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15">
+        <v>12880</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>44831.488245636574</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16">
+        <v>12865</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>44832.383314733794</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>-1305762798</v>
+      </c>
+      <c r="G17">
+        <v>12869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>44831.503006944447</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18">
+        <v>12866</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>44831.342117708336</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19">
+        <v>12864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>44830.317726655092</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20">
+        <v>12857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21" s="6">
+        <v>44832.458976122682</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21">
+        <v>12871</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>26</v>
+      </c>
+      <c r="B22" s="6">
+        <v>44835.208468900462</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22">
+        <v>12886</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6">
+        <v>44830.694514849536</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23">
+        <v>12863</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24" s="6">
+        <v>44830.618995983794</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24">
+        <v>12860</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25" s="6">
+        <v>44830.694456793979</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25">
+        <v>12862</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26" s="6">
+        <v>44832.574637997684</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26">
+        <v>12875</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{97A7C9C2-741E-4F4E-A66D-EB086C7FF489}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>